<commit_message>
update 2548 files and delete 4 files
</commit_message>
<xml_diff>
--- a/data_month/zb/交通运输/全国港口货物吞吐量（2019-）.xlsx
+++ b/data_month/zb/交通运输/全国港口货物吞吐量（2019-）.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,1892 +494,2327 @@
           <t>沿海港口货物吞吐量_累计增长</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>全国港口货物吞吐量</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>外贸货物吞吐量</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>沿海港口货物吞吐量</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2019-01</t>
+          <t>2019-10</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.9</v>
+        <v>4.2665806645</v>
       </c>
       <c r="C2" t="n">
-        <v>114129.8883</v>
+        <v>120960.739</v>
       </c>
       <c r="D2" t="n">
-        <v>114129.8883</v>
+        <v>1151066.6479</v>
       </c>
       <c r="E2" t="n">
-        <v>6.9</v>
+        <v>5.0757090148</v>
       </c>
       <c r="F2" t="n">
-        <v>5.6</v>
+        <v>7.2172251286</v>
       </c>
       <c r="G2" t="n">
-        <v>37794.8211</v>
+        <v>36825.8179</v>
       </c>
       <c r="H2" t="n">
-        <v>37794.8211</v>
+        <v>359944.2987</v>
       </c>
       <c r="I2" t="n">
-        <v>5.6</v>
+        <v>4.3038091109</v>
       </c>
       <c r="J2" t="n">
-        <v>5.8</v>
+        <v>4.6672476606</v>
       </c>
       <c r="K2" t="n">
-        <v>77791.8564</v>
+        <v>78833.069</v>
       </c>
       <c r="L2" t="n">
-        <v>77791.8564</v>
+        <v>763130.3155</v>
       </c>
       <c r="M2" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="N2" t="n">
-        <v>114129.8883</v>
-      </c>
-      <c r="O2" t="n">
-        <v>37794.8211</v>
-      </c>
-      <c r="P2" t="n">
-        <v>77791.8564</v>
+        <v>3.7278398072</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2019-02</t>
+          <t>2019-11</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1.2487667084</v>
+        <v>7.3627287402</v>
       </c>
       <c r="C3" t="n">
-        <v>88648.9289</v>
+        <v>120641.0678</v>
       </c>
       <c r="D3" t="n">
-        <v>202778.8172</v>
+        <v>1271707.7157</v>
       </c>
       <c r="E3" t="n">
-        <v>3.1838572491</v>
+        <v>5.2838957289</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.9653417083</v>
+        <v>8.2466940212</v>
       </c>
       <c r="G3" t="n">
-        <v>30424.2346</v>
+        <v>36529.3133</v>
       </c>
       <c r="H3" t="n">
-        <v>68219.0557</v>
+        <v>396473.612</v>
       </c>
       <c r="I3" t="n">
-        <v>2.1091878204</v>
+        <v>4.6549318274</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.4791024367</v>
+        <v>5.4342058015</v>
       </c>
       <c r="K3" t="n">
-        <v>62744.228</v>
+        <v>77234.08379999999</v>
       </c>
       <c r="L3" t="n">
-        <v>140672.1211</v>
+        <v>840364.3993</v>
       </c>
       <c r="M3" t="n">
-        <v>2.9759068957</v>
-      </c>
-      <c r="N3" t="n">
-        <v>88648.92889999998</v>
-      </c>
-      <c r="O3" t="n">
-        <v>30424.2346</v>
-      </c>
-      <c r="P3" t="n">
-        <v>62880.26469999999</v>
+        <v>3.8820337199</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2019-03</t>
+          <t>2019-12</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.3359091924</v>
+        <v>9.7364612289</v>
       </c>
       <c r="C4" t="n">
-        <v>112503.9467</v>
+        <v>123375.4571</v>
       </c>
       <c r="D4" t="n">
-        <v>315282.7639</v>
+        <v>1395083.1728</v>
       </c>
       <c r="E4" t="n">
-        <v>4.297416862</v>
+        <v>5.654877072</v>
       </c>
       <c r="F4" t="n">
-        <v>4.9265063749</v>
+        <v>5.7578567532</v>
       </c>
       <c r="G4" t="n">
-        <v>35613.0646</v>
+        <v>35595.7465</v>
       </c>
       <c r="H4" t="n">
-        <v>103832.1203</v>
+        <v>432069.3585</v>
       </c>
       <c r="I4" t="n">
-        <v>3.0602967905</v>
+        <v>4.7446571642</v>
       </c>
       <c r="J4" t="n">
-        <v>3.7524016222</v>
+        <v>9.014135058200001</v>
       </c>
       <c r="K4" t="n">
-        <v>75287.7164</v>
+        <v>78409.38400000001</v>
       </c>
       <c r="L4" t="n">
-        <v>215959.8375</v>
+        <v>918773.7833</v>
       </c>
       <c r="M4" t="n">
-        <v>3.2449991611</v>
-      </c>
-      <c r="N4" t="n">
-        <v>112503.9467</v>
-      </c>
-      <c r="O4" t="n">
-        <v>35613.0646</v>
-      </c>
-      <c r="P4" t="n">
-        <v>75287.7164</v>
+        <v>4.3006370931</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2019-04</t>
+          <t>2019-01</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.9713127996</v>
+        <v>6.9</v>
       </c>
       <c r="C5" t="n">
-        <v>114542.1405</v>
+        <v>114129.8883</v>
       </c>
       <c r="D5" t="n">
-        <v>429824.9044</v>
+        <v>114129.8883</v>
       </c>
       <c r="E5" t="n">
-        <v>4.2108055274</v>
+        <v>6.9</v>
       </c>
       <c r="F5" t="n">
-        <v>0.817172506</v>
+        <v>5.6</v>
       </c>
       <c r="G5" t="n">
-        <v>34524.6701</v>
+        <v>37794.8211</v>
       </c>
       <c r="H5" t="n">
-        <v>138356.7904</v>
+        <v>37794.8211</v>
       </c>
       <c r="I5" t="n">
-        <v>2.4918187523</v>
+        <v>5.6</v>
       </c>
       <c r="J5" t="n">
-        <v>2.1096993249</v>
+        <v>5.8</v>
       </c>
       <c r="K5" t="n">
-        <v>75262.5836</v>
+        <v>77791.8564</v>
       </c>
       <c r="L5" t="n">
-        <v>291222.4211</v>
+        <v>77791.8564</v>
       </c>
       <c r="M5" t="n">
-        <v>2.9490832214</v>
-      </c>
-      <c r="N5" t="n">
-        <v>114542.1405</v>
-      </c>
-      <c r="O5" t="n">
-        <v>34524.6701</v>
-      </c>
-      <c r="P5" t="n">
-        <v>75262.58359999998</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2019-05</t>
+          <t>2019-02</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.7238715366</v>
+        <v>-1.2487667084</v>
       </c>
       <c r="C6" t="n">
-        <v>120190.4009</v>
+        <v>88648.9289</v>
       </c>
       <c r="D6" t="n">
-        <v>550015.3053</v>
+        <v>202778.8172</v>
       </c>
       <c r="E6" t="n">
-        <v>4.0950973199</v>
+        <v>3.1838572491</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9498327331999999</v>
+        <v>-1.9653417083</v>
       </c>
       <c r="G6" t="n">
-        <v>36665.4277</v>
+        <v>30424.2346</v>
       </c>
       <c r="H6" t="n">
-        <v>175022.2181</v>
+        <v>68219.0557</v>
       </c>
       <c r="I6" t="n">
-        <v>2.1644912153</v>
+        <v>2.1091878204</v>
       </c>
       <c r="J6" t="n">
-        <v>1.8482839454</v>
+        <v>-0.4791024367</v>
       </c>
       <c r="K6" t="n">
-        <v>79140.19560000001</v>
+        <v>62744.228</v>
       </c>
       <c r="L6" t="n">
-        <v>370362.6167</v>
+        <v>140672.1211</v>
       </c>
       <c r="M6" t="n">
-        <v>2.7122809313</v>
-      </c>
-      <c r="N6" t="n">
-        <v>120190.4009</v>
-      </c>
-      <c r="O6" t="n">
-        <v>36665.4277</v>
-      </c>
-      <c r="P6" t="n">
-        <v>79140.19560000004</v>
+        <v>2.9759068957</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2019-06</t>
+          <t>2019-03</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6.6796207469</v>
+        <v>6.3359091924</v>
       </c>
       <c r="C7" t="n">
-        <v>121285.5351</v>
+        <v>112503.9467</v>
       </c>
       <c r="D7" t="n">
-        <v>671300.8404</v>
+        <v>315282.7639</v>
       </c>
       <c r="E7" t="n">
-        <v>4.547444496</v>
+        <v>4.297416862</v>
       </c>
       <c r="F7" t="n">
-        <v>3.5386242031</v>
+        <v>4.9265063749</v>
       </c>
       <c r="G7" t="n">
-        <v>36330.1441</v>
+        <v>35613.0646</v>
       </c>
       <c r="H7" t="n">
-        <v>211352.3622</v>
+        <v>103832.1203</v>
       </c>
       <c r="I7" t="n">
-        <v>2.3981996412</v>
+        <v>3.0602967905</v>
       </c>
       <c r="J7" t="n">
-        <v>4.6979063022</v>
+        <v>3.7524016222</v>
       </c>
       <c r="K7" t="n">
-        <v>79124.69409999999</v>
+        <v>75287.7164</v>
       </c>
       <c r="L7" t="n">
-        <v>449487.3108</v>
+        <v>215959.8375</v>
       </c>
       <c r="M7" t="n">
-        <v>3.0555117888</v>
-      </c>
-      <c r="N7" t="n">
-        <v>121285.5351</v>
-      </c>
-      <c r="O7" t="n">
-        <v>36330.1441</v>
-      </c>
-      <c r="P7" t="n">
-        <v>79124.69409999996</v>
+        <v>3.2449991611</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2019-07</t>
+          <t>2019-04</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7.1246883168</v>
+        <v>3.9713127996</v>
       </c>
       <c r="C8" t="n">
-        <v>118365.6198</v>
+        <v>114542.1405</v>
       </c>
       <c r="D8" t="n">
-        <v>789666.4602</v>
+        <v>429824.9044</v>
       </c>
       <c r="E8" t="n">
-        <v>4.9252026344</v>
+        <v>4.2108055274</v>
       </c>
       <c r="F8" t="n">
-        <v>6.6435380447</v>
+        <v>0.817172506</v>
       </c>
       <c r="G8" t="n">
-        <v>36914.1396</v>
+        <v>34524.6701</v>
       </c>
       <c r="H8" t="n">
-        <v>248266.5018</v>
+        <v>138356.7904</v>
       </c>
       <c r="I8" t="n">
-        <v>3.0076453238</v>
+        <v>2.4918187523</v>
       </c>
       <c r="J8" t="n">
-        <v>4.7540457259</v>
+        <v>2.1096993249</v>
       </c>
       <c r="K8" t="n">
-        <v>77841.39139999999</v>
+        <v>75262.5836</v>
       </c>
       <c r="L8" t="n">
-        <v>527328.7022000001</v>
+        <v>291222.4211</v>
       </c>
       <c r="M8" t="n">
-        <v>3.3024346469</v>
-      </c>
-      <c r="N8" t="n">
-        <v>118365.6198</v>
-      </c>
-      <c r="O8" t="n">
-        <v>36914.13959999999</v>
-      </c>
-      <c r="P8" t="n">
-        <v>77841.39140000008</v>
+        <v>2.9490832214</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2019-08</t>
+          <t>2019-05</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6.3819141178</v>
+        <v>3.7238715366</v>
       </c>
       <c r="C9" t="n">
-        <v>119941.1438</v>
+        <v>120190.4009</v>
       </c>
       <c r="D9" t="n">
-        <v>909607.6040000001</v>
+        <v>550015.3053</v>
       </c>
       <c r="E9" t="n">
-        <v>5.1137327202</v>
+        <v>4.0950973199</v>
       </c>
       <c r="F9" t="n">
-        <v>8.3623137844</v>
+        <v>0.9498327331999999</v>
       </c>
       <c r="G9" t="n">
-        <v>37859.4829</v>
+        <v>36665.4277</v>
       </c>
       <c r="H9" t="n">
-        <v>286125.9847</v>
+        <v>175022.2181</v>
       </c>
       <c r="I9" t="n">
-        <v>3.6856032524</v>
+        <v>2.1644912153</v>
       </c>
       <c r="J9" t="n">
-        <v>4.7115156924</v>
+        <v>1.8482839454</v>
       </c>
       <c r="K9" t="n">
-        <v>78356.7969</v>
+        <v>79140.19560000001</v>
       </c>
       <c r="L9" t="n">
-        <v>605685.4991</v>
+        <v>370362.6167</v>
       </c>
       <c r="M9" t="n">
-        <v>3.4817687647</v>
-      </c>
-      <c r="N9" t="n">
-        <v>119941.1438000001</v>
-      </c>
-      <c r="O9" t="n">
-        <v>37859.48289999997</v>
-      </c>
-      <c r="P9" t="n">
-        <v>78356.79689999996</v>
+        <v>2.7122809313</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2019-09</t>
+          <t>2019-06</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5.607477826</v>
+        <v>6.6796207469</v>
       </c>
       <c r="C10" t="n">
-        <v>120498.3049</v>
+        <v>121285.5351</v>
       </c>
       <c r="D10" t="n">
-        <v>1030105.9089</v>
+        <v>671300.8404</v>
       </c>
       <c r="E10" t="n">
-        <v>5.1707431487</v>
+        <v>4.547444496</v>
       </c>
       <c r="F10" t="n">
-        <v>6.3333476207</v>
+        <v>3.5386242031</v>
       </c>
       <c r="G10" t="n">
-        <v>36992.4961</v>
+        <v>36330.1441</v>
       </c>
       <c r="H10" t="n">
-        <v>323118.4808</v>
+        <v>211352.3622</v>
       </c>
       <c r="I10" t="n">
-        <v>3.9820617562</v>
+        <v>2.3981996412</v>
       </c>
       <c r="J10" t="n">
-        <v>4.7143536246</v>
+        <v>4.6979063022</v>
       </c>
       <c r="K10" t="n">
-        <v>78611.74739999999</v>
+        <v>79124.69409999999</v>
       </c>
       <c r="L10" t="n">
-        <v>684297.2465</v>
+        <v>449487.3108</v>
       </c>
       <c r="M10" t="n">
-        <v>3.6212342835</v>
-      </c>
-      <c r="N10" t="n">
-        <v>120498.3049</v>
-      </c>
-      <c r="O10" t="n">
-        <v>36992.49610000005</v>
-      </c>
-      <c r="P10" t="n">
-        <v>78611.74739999999</v>
+        <v>3.0555117888</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2019-10</t>
+          <t>2019-07</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.2665806645</v>
+        <v>7.1246883168</v>
       </c>
       <c r="C11" t="n">
-        <v>120960.739</v>
+        <v>118365.6198</v>
       </c>
       <c r="D11" t="n">
-        <v>1151066.6479</v>
+        <v>789666.4602</v>
       </c>
       <c r="E11" t="n">
-        <v>5.0757090148</v>
+        <v>4.9252026344</v>
       </c>
       <c r="F11" t="n">
-        <v>7.2172251286</v>
+        <v>6.6435380447</v>
       </c>
       <c r="G11" t="n">
-        <v>36825.8179</v>
+        <v>36914.1396</v>
       </c>
       <c r="H11" t="n">
-        <v>359944.2987</v>
+        <v>248266.5018</v>
       </c>
       <c r="I11" t="n">
-        <v>4.3038091109</v>
+        <v>3.0076453238</v>
       </c>
       <c r="J11" t="n">
-        <v>4.6672476606</v>
+        <v>4.7540457259</v>
       </c>
       <c r="K11" t="n">
-        <v>78833.069</v>
+        <v>77841.39139999999</v>
       </c>
       <c r="L11" t="n">
-        <v>763130.3155</v>
+        <v>527328.7022000001</v>
       </c>
       <c r="M11" t="n">
-        <v>3.7278398072</v>
-      </c>
-      <c r="N11" t="n">
-        <v>120960.7389999999</v>
-      </c>
-      <c r="O11" t="n">
-        <v>36825.81789999997</v>
-      </c>
-      <c r="P11" t="n">
-        <v>78833.06900000002</v>
+        <v>3.3024346469</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>2019-11</t>
+          <t>2019-08</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7.3627287402</v>
+        <v>6.3819141178</v>
       </c>
       <c r="C12" t="n">
-        <v>120641.0678</v>
+        <v>119941.1438</v>
       </c>
       <c r="D12" t="n">
-        <v>1271707.7157</v>
+        <v>909607.6040000001</v>
       </c>
       <c r="E12" t="n">
-        <v>5.2838957289</v>
+        <v>5.1137327202</v>
       </c>
       <c r="F12" t="n">
-        <v>8.2466940212</v>
+        <v>8.3623137844</v>
       </c>
       <c r="G12" t="n">
-        <v>36529.3133</v>
+        <v>37859.4829</v>
       </c>
       <c r="H12" t="n">
-        <v>396473.612</v>
+        <v>286125.9847</v>
       </c>
       <c r="I12" t="n">
-        <v>4.6549318274</v>
+        <v>3.6856032524</v>
       </c>
       <c r="J12" t="n">
-        <v>5.4342058015</v>
+        <v>4.7115156924</v>
       </c>
       <c r="K12" t="n">
-        <v>77234.08379999999</v>
+        <v>78356.7969</v>
       </c>
       <c r="L12" t="n">
-        <v>840364.3993</v>
+        <v>605685.4991</v>
       </c>
       <c r="M12" t="n">
-        <v>3.8820337199</v>
-      </c>
-      <c r="N12" t="n">
-        <v>120641.0678000001</v>
-      </c>
-      <c r="O12" t="n">
-        <v>36529.31330000004</v>
-      </c>
-      <c r="P12" t="n">
-        <v>77234.08380000002</v>
+        <v>3.4817687647</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>2019-12</t>
+          <t>2019-09</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9.7364612289</v>
+        <v>5.607477826</v>
       </c>
       <c r="C13" t="n">
-        <v>123375.4571</v>
+        <v>120498.3049</v>
       </c>
       <c r="D13" t="n">
-        <v>1395083.1728</v>
+        <v>1030105.9089</v>
       </c>
       <c r="E13" t="n">
-        <v>5.654877072</v>
+        <v>5.1707431487</v>
       </c>
       <c r="F13" t="n">
-        <v>5.7578567532</v>
+        <v>6.3333476207</v>
       </c>
       <c r="G13" t="n">
-        <v>35595.7465</v>
+        <v>36992.4961</v>
       </c>
       <c r="H13" t="n">
-        <v>432069.3585</v>
+        <v>323118.4808</v>
       </c>
       <c r="I13" t="n">
-        <v>4.7446571642</v>
+        <v>3.9820617562</v>
       </c>
       <c r="J13" t="n">
-        <v>9.014135058200001</v>
+        <v>4.7143536246</v>
       </c>
       <c r="K13" t="n">
-        <v>78409.38400000001</v>
+        <v>78611.74739999999</v>
       </c>
       <c r="L13" t="n">
-        <v>918773.7833</v>
+        <v>684297.2465</v>
       </c>
       <c r="M13" t="n">
-        <v>4.3006370931</v>
-      </c>
-      <c r="N13" t="n">
-        <v>123375.4571</v>
-      </c>
-      <c r="O13" t="n">
-        <v>35595.74649999995</v>
-      </c>
-      <c r="P13" t="n">
-        <v>78409.38399999996</v>
+        <v>3.6212342835</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>2020-01</t>
+          <t>2020-10</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-3.4</v>
+        <v>9.8036008196</v>
       </c>
       <c r="C14" t="n">
-        <v>110233</v>
+        <v>132819.247</v>
       </c>
       <c r="D14" t="n">
-        <v>110233</v>
+        <v>1193381.0529</v>
       </c>
       <c r="E14" t="n">
-        <v>-3.4</v>
+        <v>3.6761038188</v>
       </c>
       <c r="F14" t="n">
-        <v>1.3</v>
+        <v>6.0213644298</v>
       </c>
       <c r="G14" t="n">
-        <v>38274</v>
+        <v>39043.2346</v>
       </c>
       <c r="H14" t="n">
-        <v>38274</v>
+        <v>375757.1396</v>
       </c>
       <c r="I14" t="n">
-        <v>1.3</v>
+        <v>4.3931355371</v>
       </c>
       <c r="J14" t="n">
-        <v>-2.6</v>
+        <v>6.046646871</v>
       </c>
       <c r="K14" t="n">
-        <v>75793</v>
+        <v>83599.8263</v>
       </c>
       <c r="L14" t="n">
-        <v>75793</v>
+        <v>785609.9685</v>
       </c>
       <c r="M14" t="n">
-        <v>-2.6</v>
-      </c>
-      <c r="N14" t="n">
-        <v>110233</v>
-      </c>
-      <c r="O14" t="n">
-        <v>38274</v>
-      </c>
-      <c r="P14" t="n">
-        <v>75793</v>
+        <v>2.9457161567</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>2020-02</t>
+          <t>2020-11</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-9</v>
+        <v>9.006796771699999</v>
       </c>
       <c r="C15" t="n">
-        <v>80646.10000000001</v>
+        <v>131506.9636</v>
       </c>
       <c r="D15" t="n">
-        <v>190878.84</v>
+        <v>1324888.0165</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.9</v>
+        <v>4.181802166</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3</v>
+        <v>2.6881003536</v>
       </c>
       <c r="G15" t="n">
-        <v>30520.28</v>
+        <v>37511.2579</v>
       </c>
       <c r="H15" t="n">
-        <v>68804.39999999999</v>
+        <v>413268.3975</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9</v>
+        <v>4.236041187</v>
       </c>
       <c r="J15" t="n">
-        <v>-6.9</v>
+        <v>5.6684661546</v>
       </c>
       <c r="K15" t="n">
-        <v>58440.0912</v>
+        <v>81612.0717</v>
       </c>
       <c r="L15" t="n">
-        <v>134233.0234</v>
+        <v>867222.0402</v>
       </c>
       <c r="M15" t="n">
-        <v>-4.6</v>
-      </c>
-      <c r="N15" t="n">
-        <v>80645.84</v>
-      </c>
-      <c r="O15" t="n">
-        <v>30530.39999999999</v>
-      </c>
-      <c r="P15" t="n">
-        <v>58440.02340000001</v>
+        <v>3.1959517707</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>2020-03</t>
+          <t>2020-12</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-2.4</v>
+        <v>5.4531951963</v>
       </c>
       <c r="C16" t="n">
-        <v>109847.89</v>
+        <v>130103.3616</v>
       </c>
       <c r="D16" t="n">
-        <v>300726.72</v>
+        <v>1454991.3781</v>
       </c>
       <c r="E16" t="n">
-        <v>-4.6</v>
+        <v>4.2942389721</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.6</v>
+        <v>1.9366752148</v>
       </c>
       <c r="G16" t="n">
-        <v>35382.76</v>
+        <v>36285.1205</v>
       </c>
       <c r="H16" t="n">
-        <v>104187.16</v>
+        <v>449553.518</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3</v>
+        <v>4.0466094519</v>
       </c>
       <c r="J16" t="n">
-        <v>-2.6</v>
+        <v>3.0235803153</v>
       </c>
       <c r="K16" t="n">
-        <v>73358.1781</v>
+        <v>80780.1547</v>
       </c>
       <c r="L16" t="n">
-        <v>207591.2015</v>
+        <v>948002.1949</v>
       </c>
       <c r="M16" t="n">
-        <v>-3.9</v>
-      </c>
-      <c r="N16" t="n">
-        <v>109847.88</v>
-      </c>
-      <c r="O16" t="n">
-        <v>35382.76000000001</v>
-      </c>
-      <c r="P16" t="n">
-        <v>73358.17809999999</v>
+        <v>3.1812413601</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>2020-04</t>
+          <t>2020-01</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4.1299923149</v>
+        <v>-3.4</v>
       </c>
       <c r="C17" t="n">
-        <v>119272.7221</v>
+        <v>110233</v>
       </c>
       <c r="D17" t="n">
-        <v>419999.4447</v>
+        <v>110233</v>
       </c>
       <c r="E17" t="n">
-        <v>-2.285921453</v>
+        <v>-3.4</v>
       </c>
       <c r="F17" t="n">
-        <v>2.4148755009</v>
+        <v>1.3</v>
       </c>
       <c r="G17" t="n">
-        <v>35358.3979</v>
+        <v>38274</v>
       </c>
       <c r="H17" t="n">
-        <v>139545.5564</v>
+        <v>38274</v>
       </c>
       <c r="I17" t="n">
-        <v>0.8592032213</v>
+        <v>1.3</v>
       </c>
       <c r="J17" t="n">
-        <v>1.5985127569</v>
+        <v>-2.6</v>
       </c>
       <c r="K17" t="n">
-        <v>76465.66559999999</v>
+        <v>75793</v>
       </c>
       <c r="L17" t="n">
-        <v>284056.8671</v>
+        <v>75793</v>
       </c>
       <c r="M17" t="n">
-        <v>-2.4605090408</v>
-      </c>
-      <c r="N17" t="n">
-        <v>119272.7247</v>
-      </c>
-      <c r="O17" t="n">
-        <v>35358.3964</v>
-      </c>
-      <c r="P17" t="n">
-        <v>76465.66559999998</v>
+        <v>-2.6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>2020-05</t>
+          <t>2020-02</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4.4310667575</v>
+        <v>-9</v>
       </c>
       <c r="C18" t="n">
-        <v>125516.1178</v>
+        <v>80646.10000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>545515.5625</v>
+        <v>190878.84</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.8181122883</v>
+        <v>-5.9</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8861328515</v>
+        <v>0.3</v>
       </c>
       <c r="G18" t="n">
-        <v>36990.3321</v>
+        <v>30520.28</v>
       </c>
       <c r="H18" t="n">
-        <v>176535.8885</v>
+        <v>68804.39999999999</v>
       </c>
       <c r="I18" t="n">
-        <v>0.8648447131</v>
+        <v>0.9</v>
       </c>
       <c r="J18" t="n">
-        <v>1.9794288959</v>
+        <v>-6.9</v>
       </c>
       <c r="K18" t="n">
-        <v>80706.71950000001</v>
+        <v>58440.0912</v>
       </c>
       <c r="L18" t="n">
-        <v>364763.5866</v>
+        <v>134233.0234</v>
       </c>
       <c r="M18" t="n">
-        <v>-1.5117697758</v>
-      </c>
-      <c r="N18" t="n">
-        <v>125516.1178</v>
-      </c>
-      <c r="O18" t="n">
-        <v>36990.3321</v>
-      </c>
-      <c r="P18" t="n">
-        <v>80706.71950000001</v>
+        <v>-4.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>2020-06</t>
+          <t>2020-03</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>6.9356142866</v>
+        <v>-2.4</v>
       </c>
       <c r="C19" t="n">
-        <v>129697.432</v>
+        <v>109847.89</v>
       </c>
       <c r="D19" t="n">
-        <v>675212.9945</v>
+        <v>300726.72</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5827721142</v>
+        <v>-4.6</v>
       </c>
       <c r="F19" t="n">
-        <v>8.396081754000001</v>
+        <v>-0.6</v>
       </c>
       <c r="G19" t="n">
-        <v>39380.4527</v>
+        <v>35382.76</v>
       </c>
       <c r="H19" t="n">
-        <v>215916.3412</v>
+        <v>104187.16</v>
       </c>
       <c r="I19" t="n">
-        <v>2.1594170761</v>
+        <v>0.3</v>
       </c>
       <c r="J19" t="n">
-        <v>7.5591321623</v>
+        <v>-2.6</v>
       </c>
       <c r="K19" t="n">
-        <v>85105.8343</v>
+        <v>73358.1781</v>
       </c>
       <c r="L19" t="n">
-        <v>449869.4209</v>
+        <v>207591.2015</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0850102085</v>
-      </c>
-      <c r="N19" t="n">
-        <v>129697.432</v>
-      </c>
-      <c r="O19" t="n">
-        <v>39380.45269999999</v>
-      </c>
-      <c r="P19" t="n">
-        <v>85105.83430000005</v>
+        <v>-3.9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>2020-07</t>
+          <t>2020-04</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6.0083442405</v>
+        <v>4.1299923149</v>
       </c>
       <c r="C20" t="n">
-        <v>125477.4337</v>
+        <v>119272.7221</v>
       </c>
       <c r="D20" t="n">
-        <v>800690.4282</v>
+        <v>419999.4447</v>
       </c>
       <c r="E20" t="n">
-        <v>1.3960283937</v>
+        <v>-2.285921453</v>
       </c>
       <c r="F20" t="n">
-        <v>10.0450319043</v>
+        <v>2.4148755009</v>
       </c>
       <c r="G20" t="n">
-        <v>40622.1767</v>
+        <v>35358.3979</v>
       </c>
       <c r="H20" t="n">
-        <v>256538.5179</v>
+        <v>139545.5564</v>
       </c>
       <c r="I20" t="n">
-        <v>3.3319098791</v>
+        <v>0.8592032213</v>
       </c>
       <c r="J20" t="n">
-        <v>9.759693992300001</v>
+        <v>1.5985127569</v>
       </c>
       <c r="K20" t="n">
-        <v>85438.473</v>
+        <v>76465.66559999999</v>
       </c>
       <c r="L20" t="n">
-        <v>535307.8939</v>
+        <v>284056.8671</v>
       </c>
       <c r="M20" t="n">
-        <v>1.5131343442</v>
-      </c>
-      <c r="N20" t="n">
-        <v>125477.4336999999</v>
-      </c>
-      <c r="O20" t="n">
-        <v>40622.17670000001</v>
-      </c>
-      <c r="P20" t="n">
-        <v>85438.473</v>
+        <v>-2.4605090408</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>2020-08</t>
+          <t>2020-05</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>7.2287737346</v>
+        <v>4.4310667575</v>
       </c>
       <c r="C21" t="n">
-        <v>128611.4177</v>
+        <v>125516.1178</v>
       </c>
       <c r="D21" t="n">
-        <v>929301.8459</v>
+        <v>545515.5625</v>
       </c>
       <c r="E21" t="n">
-        <v>2.1651360228</v>
+        <v>-0.8181122883</v>
       </c>
       <c r="F21" t="n">
-        <v>5.896993115</v>
+        <v>0.8861328515</v>
       </c>
       <c r="G21" t="n">
-        <v>40092.054</v>
+        <v>36990.3321</v>
       </c>
       <c r="H21" t="n">
-        <v>296630.5719</v>
+        <v>176535.8885</v>
       </c>
       <c r="I21" t="n">
-        <v>3.6713153512</v>
+        <v>0.8648447131</v>
       </c>
       <c r="J21" t="n">
-        <v>6.6217055894</v>
+        <v>1.9794288959</v>
       </c>
       <c r="K21" t="n">
-        <v>83545.3533</v>
+        <v>80706.71950000001</v>
       </c>
       <c r="L21" t="n">
-        <v>618853.2472</v>
+        <v>364763.5866</v>
       </c>
       <c r="M21" t="n">
-        <v>2.1740239975</v>
-      </c>
-      <c r="N21" t="n">
-        <v>128611.4177</v>
-      </c>
-      <c r="O21" t="n">
-        <v>40092.05399999997</v>
-      </c>
-      <c r="P21" t="n">
-        <v>83545.35329999996</v>
+        <v>-1.5117697758</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>2020-09</t>
+          <t>2020-06</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>8.930959741700001</v>
+        <v>6.9356142866</v>
       </c>
       <c r="C22" t="n">
-        <v>131259.96</v>
+        <v>129697.432</v>
       </c>
       <c r="D22" t="n">
-        <v>1060561.8059</v>
+        <v>675212.9945</v>
       </c>
       <c r="E22" t="n">
-        <v>2.9565791961</v>
+        <v>0.5827721142</v>
       </c>
       <c r="F22" t="n">
-        <v>8.3553080377</v>
+        <v>8.396081754000001</v>
       </c>
       <c r="G22" t="n">
-        <v>40083.3331</v>
+        <v>39380.4527</v>
       </c>
       <c r="H22" t="n">
-        <v>336713.905</v>
+        <v>215916.3412</v>
       </c>
       <c r="I22" t="n">
-        <v>4.2075662668</v>
+        <v>2.1594170761</v>
       </c>
       <c r="J22" t="n">
-        <v>5.781766403</v>
+        <v>7.5591321623</v>
       </c>
       <c r="K22" t="n">
-        <v>83156.895</v>
+        <v>85105.8343</v>
       </c>
       <c r="L22" t="n">
-        <v>702010.1422</v>
+        <v>449869.4209</v>
       </c>
       <c r="M22" t="n">
-        <v>2.5884797565</v>
-      </c>
-      <c r="N22" t="n">
-        <v>131259.9600000001</v>
-      </c>
-      <c r="O22" t="n">
-        <v>40083.33310000005</v>
-      </c>
-      <c r="P22" t="n">
-        <v>83156.89500000002</v>
+        <v>0.0850102085</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>2020-10</t>
+          <t>2020-07</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>9.8036008196</v>
+        <v>6.0083442405</v>
       </c>
       <c r="C23" t="n">
-        <v>132819.247</v>
+        <v>125477.4337</v>
       </c>
       <c r="D23" t="n">
-        <v>1193381.0529</v>
+        <v>800690.4282</v>
       </c>
       <c r="E23" t="n">
-        <v>3.6761038188</v>
+        <v>1.3960283937</v>
       </c>
       <c r="F23" t="n">
-        <v>6.0213644298</v>
+        <v>10.0450319043</v>
       </c>
       <c r="G23" t="n">
-        <v>39043.2346</v>
+        <v>40622.1767</v>
       </c>
       <c r="H23" t="n">
-        <v>375757.1396</v>
+        <v>256538.5179</v>
       </c>
       <c r="I23" t="n">
-        <v>4.3931355371</v>
+        <v>3.3319098791</v>
       </c>
       <c r="J23" t="n">
-        <v>6.046646871</v>
+        <v>9.759693992300001</v>
       </c>
       <c r="K23" t="n">
-        <v>83599.8263</v>
+        <v>85438.473</v>
       </c>
       <c r="L23" t="n">
-        <v>785609.9685</v>
+        <v>535307.8939</v>
       </c>
       <c r="M23" t="n">
-        <v>2.9457161567</v>
-      </c>
-      <c r="N23" t="n">
-        <v>132819.247</v>
-      </c>
-      <c r="O23" t="n">
-        <v>39043.23459999997</v>
-      </c>
-      <c r="P23" t="n">
-        <v>83599.82629999996</v>
+        <v>1.5131343442</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>2020-11</t>
+          <t>2020-08</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>9.006796771699999</v>
+        <v>7.2287737346</v>
       </c>
       <c r="C24" t="n">
-        <v>131506.9636</v>
+        <v>128611.4177</v>
       </c>
       <c r="D24" t="n">
-        <v>1324888.0165</v>
+        <v>929301.8459</v>
       </c>
       <c r="E24" t="n">
-        <v>4.181802166</v>
+        <v>2.1651360228</v>
       </c>
       <c r="F24" t="n">
-        <v>2.6881003536</v>
+        <v>5.896993115</v>
       </c>
       <c r="G24" t="n">
-        <v>37511.2579</v>
+        <v>40092.054</v>
       </c>
       <c r="H24" t="n">
-        <v>413268.3975</v>
+        <v>296630.5719</v>
       </c>
       <c r="I24" t="n">
-        <v>4.236041187</v>
+        <v>3.6713153512</v>
       </c>
       <c r="J24" t="n">
-        <v>5.6684661546</v>
+        <v>6.6217055894</v>
       </c>
       <c r="K24" t="n">
-        <v>81612.0717</v>
+        <v>83545.3533</v>
       </c>
       <c r="L24" t="n">
-        <v>867222.0402</v>
+        <v>618853.2472</v>
       </c>
       <c r="M24" t="n">
-        <v>3.1959517707</v>
-      </c>
-      <c r="N24" t="n">
-        <v>131506.9635999999</v>
-      </c>
-      <c r="O24" t="n">
-        <v>37511.25790000003</v>
-      </c>
-      <c r="P24" t="n">
-        <v>81612.07170000009</v>
+        <v>2.1740239975</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>2020-12</t>
+          <t>2020-09</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5.4531951963</v>
+        <v>8.930959741700001</v>
       </c>
       <c r="C25" t="n">
-        <v>130103.3616</v>
+        <v>131259.96</v>
       </c>
       <c r="D25" t="n">
-        <v>1454991.3781</v>
+        <v>1060561.8059</v>
       </c>
       <c r="E25" t="n">
-        <v>4.2942389721</v>
+        <v>2.9565791961</v>
       </c>
       <c r="F25" t="n">
-        <v>1.9366752148</v>
+        <v>8.3553080377</v>
       </c>
       <c r="G25" t="n">
-        <v>36285.1205</v>
+        <v>40083.3331</v>
       </c>
       <c r="H25" t="n">
-        <v>449553.518</v>
+        <v>336713.905</v>
       </c>
       <c r="I25" t="n">
-        <v>4.0466094519</v>
+        <v>4.2075662668</v>
       </c>
       <c r="J25" t="n">
-        <v>3.0235803153</v>
+        <v>5.781766403</v>
       </c>
       <c r="K25" t="n">
-        <v>80780.1547</v>
+        <v>83156.895</v>
       </c>
       <c r="L25" t="n">
-        <v>948002.1949</v>
+        <v>702010.1422</v>
       </c>
       <c r="M25" t="n">
-        <v>3.1812413601</v>
-      </c>
-      <c r="N25" t="n">
-        <v>130103.3616000002</v>
-      </c>
-      <c r="O25" t="n">
-        <v>36285.12049999996</v>
-      </c>
-      <c r="P25" t="n">
-        <v>80780.15469999996</v>
+        <v>2.5884797565</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>2021-01</t>
+          <t>2021-10</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>17.3623467689</v>
+        <v>-0.5134546501</v>
       </c>
       <c r="C26" t="n">
-        <v>129371.7213</v>
+        <v>132137.2804</v>
       </c>
       <c r="D26" t="n">
-        <v>129371.7213</v>
+        <v>1286973.9779</v>
       </c>
       <c r="E26" t="n">
-        <v>17.3623467689</v>
+        <v>7.8426689256</v>
       </c>
       <c r="F26" t="n">
-        <v>6.6307762586</v>
+        <v>0.5310907309</v>
       </c>
       <c r="G26" t="n">
-        <v>40822.6537</v>
+        <v>39250.5896</v>
       </c>
       <c r="H26" t="n">
-        <v>40822.6537</v>
+        <v>393310.3352</v>
       </c>
       <c r="I26" t="n">
-        <v>6.6307762586</v>
+        <v>4.6714203804</v>
       </c>
       <c r="J26" t="n">
-        <v>10.7614767805</v>
+        <v>0.5954721703</v>
       </c>
       <c r="K26" t="n">
-        <v>83949.371</v>
+        <v>84097.64</v>
       </c>
       <c r="L26" t="n">
-        <v>83949.371</v>
+        <v>830203.7202</v>
       </c>
       <c r="M26" t="n">
-        <v>10.7614767805</v>
-      </c>
-      <c r="N26" t="n">
-        <v>129371.7213</v>
-      </c>
-      <c r="O26" t="n">
-        <v>40822.6537</v>
-      </c>
-      <c r="P26" t="n">
-        <v>83949.371</v>
+        <v>5.6763220285</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>2021-02</t>
+          <t>2021-11</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>24.4270311875</v>
+        <v>1.7324554819</v>
       </c>
       <c r="C27" t="n">
-        <v>100345.5531</v>
+        <v>133785.2632</v>
       </c>
       <c r="D27" t="n">
-        <v>229717.2744</v>
+        <v>1420759.2411</v>
       </c>
       <c r="E27" t="n">
-        <v>20.3471683782</v>
+        <v>7.2361756923</v>
       </c>
       <c r="F27" t="n">
-        <v>16.7944309627</v>
+        <v>4.2115908355</v>
       </c>
       <c r="G27" t="n">
-        <v>35645.9835</v>
+        <v>39091.0786</v>
       </c>
       <c r="H27" t="n">
-        <v>76468.6372</v>
+        <v>432401.4138</v>
       </c>
       <c r="I27" t="n">
-        <v>11.1391735622</v>
+        <v>4.6296828927</v>
       </c>
       <c r="J27" t="n">
-        <v>18.2190429231</v>
+        <v>2.5255032216</v>
       </c>
       <c r="K27" t="n">
-        <v>69087.3165</v>
+        <v>83673.1872</v>
       </c>
       <c r="L27" t="n">
-        <v>153036.6875</v>
+        <v>913876.9074</v>
       </c>
       <c r="M27" t="n">
-        <v>14.0082251176</v>
-      </c>
-      <c r="N27" t="n">
-        <v>100345.5531</v>
-      </c>
-      <c r="O27" t="n">
-        <v>35645.98349999999</v>
-      </c>
-      <c r="P27" t="n">
-        <v>69087.3165</v>
+        <v>5.3798064437</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>2021-03</t>
+          <t>2021-12</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>16.234042078</v>
+        <v>2.822148217</v>
       </c>
       <c r="C28" t="n">
-        <v>127680.6385</v>
+        <v>133775.07</v>
       </c>
       <c r="D28" t="n">
-        <v>357397.9129</v>
+        <v>1554534.31</v>
       </c>
       <c r="E28" t="n">
-        <v>18.844747088</v>
+        <v>6.841479324</v>
       </c>
       <c r="F28" t="n">
-        <v>11.8767708199</v>
+        <v>2.892953049</v>
       </c>
       <c r="G28" t="n">
-        <v>39585.092</v>
+        <v>37334.83</v>
       </c>
       <c r="H28" t="n">
-        <v>116053.7292</v>
+        <v>469736.25</v>
       </c>
       <c r="I28" t="n">
-        <v>11.3896672784</v>
+        <v>4.489505029</v>
       </c>
       <c r="J28" t="n">
-        <v>14.7251150175</v>
+        <v>3.221026637</v>
       </c>
       <c r="K28" t="n">
-        <v>84160.2542</v>
+        <v>83382.11</v>
       </c>
       <c r="L28" t="n">
-        <v>237196.9417</v>
+        <v>997259.01</v>
       </c>
       <c r="M28" t="n">
-        <v>14.2615582867</v>
-      </c>
-      <c r="N28" t="n">
-        <v>127680.6385</v>
-      </c>
-      <c r="O28" t="n">
-        <v>39585.092</v>
-      </c>
-      <c r="P28" t="n">
-        <v>84160.2542</v>
+        <v>5.195854795</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>2021-04</t>
+          <t>2021-01</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>10.9468446516</v>
+        <v>17.3623467689</v>
       </c>
       <c r="C29" t="n">
-        <v>132329.3217</v>
+        <v>129371.7213</v>
       </c>
       <c r="D29" t="n">
-        <v>489727.2346</v>
+        <v>129371.7213</v>
       </c>
       <c r="E29" t="n">
-        <v>16.6018766881</v>
+        <v>17.3623467689</v>
       </c>
       <c r="F29" t="n">
-        <v>10.3764554332</v>
+        <v>6.6307762586</v>
       </c>
       <c r="G29" t="n">
-        <v>39027.3463</v>
+        <v>40822.6537</v>
       </c>
       <c r="H29" t="n">
-        <v>155081.0755</v>
+        <v>40822.6537</v>
       </c>
       <c r="I29" t="n">
-        <v>11.1329371574</v>
+        <v>6.6307762586</v>
       </c>
       <c r="J29" t="n">
-        <v>11.1482534457</v>
+        <v>10.7614767805</v>
       </c>
       <c r="K29" t="n">
-        <v>84990.2518</v>
+        <v>83949.371</v>
       </c>
       <c r="L29" t="n">
-        <v>322187.1935</v>
+        <v>83949.371</v>
       </c>
       <c r="M29" t="n">
-        <v>13.4234833994</v>
-      </c>
-      <c r="N29" t="n">
-        <v>132329.3217</v>
-      </c>
-      <c r="O29" t="n">
-        <v>39027.3463</v>
-      </c>
-      <c r="P29" t="n">
-        <v>84990.2518</v>
+        <v>10.7614767805</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>2021-05</t>
+          <t>2021-02</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10.3324585936</v>
+        <v>24.4270311875</v>
       </c>
       <c r="C30" t="n">
-        <v>138485.0187</v>
+        <v>100345.5531</v>
       </c>
       <c r="D30" t="n">
-        <v>628212.2533</v>
+        <v>229717.2744</v>
       </c>
       <c r="E30" t="n">
-        <v>15.159364184</v>
+        <v>20.3471683782</v>
       </c>
       <c r="F30" t="n">
-        <v>8.830799332</v>
+        <v>16.7944309627</v>
       </c>
       <c r="G30" t="n">
-        <v>40256.8741</v>
+        <v>35645.9835</v>
       </c>
       <c r="H30" t="n">
-        <v>195337.9496</v>
+        <v>76468.6372</v>
       </c>
       <c r="I30" t="n">
-        <v>10.6505602117</v>
+        <v>11.1391735622</v>
       </c>
       <c r="J30" t="n">
-        <v>8.9377489814</v>
+        <v>18.2190429231</v>
       </c>
       <c r="K30" t="n">
-        <v>87920.08349999999</v>
+        <v>69087.3165</v>
       </c>
       <c r="L30" t="n">
-        <v>410107.277</v>
+        <v>153036.6875</v>
       </c>
       <c r="M30" t="n">
-        <v>12.4309805216</v>
-      </c>
-      <c r="N30" t="n">
-        <v>138485.0187</v>
-      </c>
-      <c r="O30" t="n">
-        <v>40256.87409999999</v>
-      </c>
-      <c r="P30" t="n">
-        <v>87920.08350000001</v>
+        <v>14.0082251176</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>2021-06</t>
+          <t>2021-03</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4.9533909045</v>
+        <v>16.234042078</v>
       </c>
       <c r="C31" t="n">
-        <v>136121.8528</v>
+        <v>127680.6385</v>
       </c>
       <c r="D31" t="n">
-        <v>764334.1061</v>
+        <v>357397.9129</v>
       </c>
       <c r="E31" t="n">
-        <v>13.198962746</v>
+        <v>18.844747088</v>
       </c>
       <c r="F31" t="n">
-        <v>2.5428780812</v>
+        <v>11.8767708199</v>
       </c>
       <c r="G31" t="n">
-        <v>40381.8496</v>
+        <v>39585.092</v>
       </c>
       <c r="H31" t="n">
-        <v>235719.7992</v>
+        <v>116053.7292</v>
       </c>
       <c r="I31" t="n">
-        <v>9.171819923399999</v>
+        <v>11.3896672784</v>
       </c>
       <c r="J31" t="n">
-        <v>1.2929500181</v>
+        <v>14.7251150175</v>
       </c>
       <c r="K31" t="n">
-        <v>86206.2102</v>
+        <v>84160.2542</v>
       </c>
       <c r="L31" t="n">
-        <v>496313.4872</v>
+        <v>237196.9417</v>
       </c>
       <c r="M31" t="n">
-        <v>10.3238993678</v>
-      </c>
-      <c r="N31" t="n">
-        <v>136121.8528</v>
-      </c>
-      <c r="O31" t="n">
-        <v>40381.84960000002</v>
-      </c>
-      <c r="P31" t="n">
-        <v>86206.21019999997</v>
+        <v>14.2615582867</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>2021-07</t>
+          <t>2021-04</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1.0308186595</v>
+        <v>10.9468446516</v>
       </c>
       <c r="C32" t="n">
-        <v>126770.8785</v>
+        <v>132329.3217</v>
       </c>
       <c r="D32" t="n">
-        <v>891104.9846</v>
+        <v>489727.2346</v>
       </c>
       <c r="E32" t="n">
-        <v>11.292074092</v>
+        <v>16.6018766881</v>
       </c>
       <c r="F32" t="n">
-        <v>-4.734977188</v>
+        <v>10.3764554332</v>
       </c>
       <c r="G32" t="n">
-        <v>38698.7259</v>
+        <v>39027.3463</v>
       </c>
       <c r="H32" t="n">
-        <v>274418.5251</v>
+        <v>155081.0755</v>
       </c>
       <c r="I32" t="n">
-        <v>6.9697164178</v>
+        <v>11.1329371574</v>
       </c>
       <c r="J32" t="n">
-        <v>-4.2251020802</v>
+        <v>11.1482534457</v>
       </c>
       <c r="K32" t="n">
-        <v>81828.6103</v>
+        <v>84990.2518</v>
       </c>
       <c r="L32" t="n">
-        <v>578142.0975</v>
+        <v>322187.1935</v>
       </c>
       <c r="M32" t="n">
-        <v>8.001788146199999</v>
-      </c>
-      <c r="N32" t="n">
-        <v>126770.8785</v>
-      </c>
-      <c r="O32" t="n">
-        <v>38698.72590000002</v>
-      </c>
-      <c r="P32" t="n">
-        <v>81828.61030000006</v>
+        <v>13.4234833994</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>2021-08</t>
+          <t>2021-05</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>4.9088770755</v>
+        <v>10.3324585936</v>
       </c>
       <c r="C33" t="n">
-        <v>134924.7941</v>
+        <v>138485.0187</v>
       </c>
       <c r="D33" t="n">
-        <v>1026029.7787</v>
+        <v>628212.2533</v>
       </c>
       <c r="E33" t="n">
-        <v>10.4086668101</v>
+        <v>15.159364184</v>
       </c>
       <c r="F33" t="n">
-        <v>1.9711521889</v>
+        <v>8.830799332</v>
       </c>
       <c r="G33" t="n">
-        <v>40882.3294</v>
+        <v>40256.8741</v>
       </c>
       <c r="H33" t="n">
-        <v>315300.8545</v>
+        <v>195337.9496</v>
       </c>
       <c r="I33" t="n">
-        <v>6.2941194768</v>
+        <v>10.6505602117</v>
       </c>
       <c r="J33" t="n">
-        <v>3.0159467887</v>
+        <v>8.9377489814</v>
       </c>
       <c r="K33" t="n">
-        <v>86065.0367</v>
+        <v>87920.08349999999</v>
       </c>
       <c r="L33" t="n">
-        <v>664207.1342</v>
+        <v>410107.277</v>
       </c>
       <c r="M33" t="n">
-        <v>7.3286982342</v>
-      </c>
-      <c r="N33" t="n">
-        <v>134924.7941000001</v>
-      </c>
-      <c r="O33" t="n">
-        <v>40882.32939999999</v>
-      </c>
-      <c r="P33" t="n">
-        <v>86065.03669999994</v>
+        <v>12.4309805216</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>2021-09</t>
+          <t>2021-06</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-1.868841953</v>
+        <v>4.9533909045</v>
       </c>
       <c r="C34" t="n">
-        <v>128806.9188</v>
+        <v>136121.8528</v>
       </c>
       <c r="D34" t="n">
-        <v>1154836.6975</v>
+        <v>764334.1061</v>
       </c>
       <c r="E34" t="n">
-        <v>8.889146401</v>
+        <v>13.198962746</v>
       </c>
       <c r="F34" t="n">
-        <v>-3.3042212251</v>
+        <v>2.5428780812</v>
       </c>
       <c r="G34" t="n">
-        <v>38758.8911</v>
+        <v>40381.8496</v>
       </c>
       <c r="H34" t="n">
-        <v>354059.7456</v>
+        <v>235719.7992</v>
       </c>
       <c r="I34" t="n">
-        <v>5.1515070635</v>
+        <v>9.171819923399999</v>
       </c>
       <c r="J34" t="n">
-        <v>-1.5127416674</v>
+        <v>1.2929500181</v>
       </c>
       <c r="K34" t="n">
-        <v>81898.946</v>
+        <v>86206.2102</v>
       </c>
       <c r="L34" t="n">
-        <v>746106.0802</v>
+        <v>496313.4872</v>
       </c>
       <c r="M34" t="n">
-        <v>6.2813818988</v>
-      </c>
-      <c r="N34" t="n">
-        <v>128806.9188</v>
-      </c>
-      <c r="O34" t="n">
-        <v>38758.89110000001</v>
-      </c>
-      <c r="P34" t="n">
-        <v>81898.946</v>
+        <v>10.3238993678</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>2021-10</t>
+          <t>2021-07</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.5134546501</v>
+        <v>1.0308186595</v>
       </c>
       <c r="C35" t="n">
-        <v>132137.2804</v>
+        <v>126770.8785</v>
       </c>
       <c r="D35" t="n">
-        <v>1286973.9779</v>
+        <v>891104.9846</v>
       </c>
       <c r="E35" t="n">
-        <v>7.8426689256</v>
+        <v>11.292074092</v>
       </c>
       <c r="F35" t="n">
-        <v>0.5310907309</v>
+        <v>-4.734977188</v>
       </c>
       <c r="G35" t="n">
-        <v>39250.5896</v>
+        <v>38698.7259</v>
       </c>
       <c r="H35" t="n">
-        <v>393310.3352</v>
+        <v>274418.5251</v>
       </c>
       <c r="I35" t="n">
-        <v>4.6714203804</v>
+        <v>6.9697164178</v>
       </c>
       <c r="J35" t="n">
-        <v>0.5954721703</v>
+        <v>-4.2251020802</v>
       </c>
       <c r="K35" t="n">
-        <v>84097.64</v>
+        <v>81828.6103</v>
       </c>
       <c r="L35" t="n">
-        <v>830203.7202</v>
+        <v>578142.0975</v>
       </c>
       <c r="M35" t="n">
-        <v>5.6763220285</v>
-      </c>
-      <c r="N35" t="n">
-        <v>132137.2804</v>
-      </c>
-      <c r="O35" t="n">
-        <v>39250.58959999995</v>
-      </c>
-      <c r="P35" t="n">
-        <v>84097.64000000001</v>
+        <v>8.001788146199999</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>2021-11</t>
+          <t>2021-08</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1.7324554819</v>
+        <v>4.9088770755</v>
       </c>
       <c r="C36" t="n">
-        <v>133785.2632</v>
+        <v>134924.7941</v>
       </c>
       <c r="D36" t="n">
-        <v>1420759.2411</v>
+        <v>1026029.7787</v>
       </c>
       <c r="E36" t="n">
-        <v>7.2361756923</v>
+        <v>10.4086668101</v>
       </c>
       <c r="F36" t="n">
-        <v>4.2115908355</v>
+        <v>1.9711521889</v>
       </c>
       <c r="G36" t="n">
-        <v>39091.0786</v>
+        <v>40882.3294</v>
       </c>
       <c r="H36" t="n">
-        <v>432401.4138</v>
+        <v>315300.8545</v>
       </c>
       <c r="I36" t="n">
-        <v>4.6296828927</v>
+        <v>6.2941194768</v>
       </c>
       <c r="J36" t="n">
-        <v>2.5255032216</v>
+        <v>3.0159467887</v>
       </c>
       <c r="K36" t="n">
-        <v>83673.1872</v>
+        <v>86065.0367</v>
       </c>
       <c r="L36" t="n">
-        <v>913876.9074</v>
+        <v>664207.1342</v>
       </c>
       <c r="M36" t="n">
-        <v>5.3798064437</v>
-      </c>
-      <c r="N36" t="n">
-        <v>133785.2631999999</v>
-      </c>
-      <c r="O36" t="n">
-        <v>39091.07860000001</v>
-      </c>
-      <c r="P36" t="n">
-        <v>83673.18720000004</v>
+        <v>7.3286982342</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>2021-12</t>
+          <t>2021-09</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2.822148217</v>
+        <v>-1.868841953</v>
       </c>
       <c r="C37" t="n">
-        <v>133775.07</v>
+        <v>128806.9188</v>
       </c>
       <c r="D37" t="n">
-        <v>1554534.31</v>
+        <v>1154836.6975</v>
       </c>
       <c r="E37" t="n">
-        <v>6.841479324</v>
+        <v>8.889146401</v>
       </c>
       <c r="F37" t="n">
-        <v>2.892953049</v>
+        <v>-3.3042212251</v>
       </c>
       <c r="G37" t="n">
-        <v>37334.83</v>
+        <v>38758.8911</v>
       </c>
       <c r="H37" t="n">
-        <v>469736.25</v>
+        <v>354059.7456</v>
       </c>
       <c r="I37" t="n">
-        <v>4.489505029</v>
+        <v>5.1515070635</v>
       </c>
       <c r="J37" t="n">
-        <v>3.221026637</v>
+        <v>-1.5127416674</v>
       </c>
       <c r="K37" t="n">
-        <v>83382.11</v>
+        <v>81898.946</v>
       </c>
       <c r="L37" t="n">
-        <v>997259.01</v>
+        <v>746106.0802</v>
       </c>
       <c r="M37" t="n">
-        <v>5.195854795</v>
-      </c>
-      <c r="N37" t="n">
-        <v>133775.0689000001</v>
-      </c>
-      <c r="O37" t="n">
-        <v>37334.83620000002</v>
-      </c>
-      <c r="P37" t="n">
-        <v>83382.10259999998</v>
+        <v>6.2813818988</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>2022-10</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>4.3787516154</v>
+      </c>
+      <c r="C38" t="n">
+        <v>137923.2437</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1293377.1144</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.4975342633</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.2189006608</v>
+      </c>
+      <c r="G38" t="n">
+        <v>39336.5094</v>
+      </c>
+      <c r="H38" t="n">
+        <v>381580.5182</v>
+      </c>
+      <c r="I38" t="n">
+        <v>-2.9823312408</v>
+      </c>
+      <c r="J38" t="n">
+        <v>3.7136200255</v>
+      </c>
+      <c r="K38" t="n">
+        <v>87220.7068</v>
+      </c>
+      <c r="L38" t="n">
+        <v>840044.9602</v>
+      </c>
+      <c r="M38" t="n">
+        <v>1.1854006144</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>2022-11</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>3.1009293556</v>
+      </c>
+      <c r="C39" t="n">
+        <v>137933.8497</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1431310.9641</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.7426819897</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2.4158581288</v>
+      </c>
+      <c r="G39" t="n">
+        <v>40035.4636</v>
+      </c>
+      <c r="H39" t="n">
+        <v>421615.9818</v>
+      </c>
+      <c r="I39" t="n">
+        <v>-2.4943100683</v>
+      </c>
+      <c r="J39" t="n">
+        <v>4.1035886344</v>
+      </c>
+      <c r="K39" t="n">
+        <v>87106.79059999999</v>
+      </c>
+      <c r="L39" t="n">
+        <v>927151.7508</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1.4525854951</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>2022-12</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>2.5166865301</v>
+      </c>
+      <c r="C40" t="n">
+        <v>137141.7705</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1568452.7346</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.8953435179</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4.7595794726</v>
+      </c>
+      <c r="G40" t="n">
+        <v>39111.813</v>
+      </c>
+      <c r="H40" t="n">
+        <v>460727.7948</v>
+      </c>
+      <c r="I40" t="n">
+        <v>-1.9177679135</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3.0793841197</v>
+      </c>
+      <c r="K40" t="n">
+        <v>85949.76029999999</v>
+      </c>
+      <c r="L40" t="n">
+        <v>1013101.5111</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1.5886042145</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>2022-01</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.5720282551</v>
+      </c>
+      <c r="C41" t="n">
+        <v>130111.7641</v>
+      </c>
+      <c r="D41" t="n">
+        <v>130111.7641</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.5720282551</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-2.3927435173</v>
+      </c>
+      <c r="G41" t="n">
+        <v>39845.8723</v>
+      </c>
+      <c r="H41" t="n">
+        <v>39845.8723</v>
+      </c>
+      <c r="I41" t="n">
+        <v>-2.3927435173</v>
+      </c>
+      <c r="J41" t="n">
+        <v>2.6133275019</v>
+      </c>
+      <c r="K41" t="n">
+        <v>86143.243</v>
+      </c>
+      <c r="L41" t="n">
+        <v>86143.243</v>
+      </c>
+      <c r="M41" t="n">
+        <v>2.6133275019</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C42" t="n">
+        <v>105695</v>
+      </c>
+      <c r="D42" t="n">
+        <v>235807</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-5.7</v>
+      </c>
+      <c r="G42" t="n">
+        <v>33620</v>
+      </c>
+      <c r="H42" t="n">
+        <v>73465</v>
+      </c>
+      <c r="I42" t="n">
+        <v>-3.9</v>
+      </c>
+      <c r="J42" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="K42" t="n">
+        <v>70987</v>
+      </c>
+      <c r="L42" t="n">
+        <v>157130</v>
+      </c>
+      <c r="M42" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>2022-03</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>-0.3117490676</v>
+      </c>
+      <c r="C43" t="n">
+        <v>127282.5953</v>
+      </c>
+      <c r="D43" t="n">
+        <v>363089.6203</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1.5925407493</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-6.1393660523</v>
+      </c>
+      <c r="G43" t="n">
+        <v>37154.8183</v>
+      </c>
+      <c r="H43" t="n">
+        <v>110620.2064</v>
+      </c>
+      <c r="I43" t="n">
+        <v>-4.6819028027</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.2639408615</v>
+      </c>
+      <c r="K43" t="n">
+        <v>84382.3875</v>
+      </c>
+      <c r="L43" t="n">
+        <v>241512.7518</v>
+      </c>
+      <c r="M43" t="n">
+        <v>1.8195049519</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>2022-04</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>-3.7168823484</v>
+      </c>
+      <c r="C44" t="n">
+        <v>127410.7965</v>
+      </c>
+      <c r="D44" t="n">
+        <v>490500.4168</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.1578801719</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-2.6249988716</v>
+      </c>
+      <c r="G44" t="n">
+        <v>38002.8789</v>
+      </c>
+      <c r="H44" t="n">
+        <v>148623.0853</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-4.1642670965</v>
+      </c>
+      <c r="J44" t="n">
+        <v>-2.7614248108</v>
+      </c>
+      <c r="K44" t="n">
+        <v>82643.30989999999</v>
+      </c>
+      <c r="L44" t="n">
+        <v>324156.0617</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0.611094494</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>2022-05</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>-2.8024873278</v>
+      </c>
+      <c r="C45" t="n">
+        <v>134603.9936</v>
+      </c>
+      <c r="D45" t="n">
+        <v>625104.4104000001</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.4947122384</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-1.8344712959</v>
+      </c>
+      <c r="G45" t="n">
+        <v>39518.3733</v>
+      </c>
+      <c r="H45" t="n">
+        <v>188141.4586</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-3.6841233435</v>
+      </c>
+      <c r="J45" t="n">
+        <v>-1.8590614737</v>
+      </c>
+      <c r="K45" t="n">
+        <v>86285.59510000001</v>
+      </c>
+      <c r="L45" t="n">
+        <v>410441.6568</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0.0815347151</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>2022-06</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>-2.3121882602</v>
+      </c>
+      <c r="C46" t="n">
+        <v>132974.4593</v>
+      </c>
+      <c r="D46" t="n">
+        <v>758078.8697</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-0.8183903283</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-3.7842773799</v>
+      </c>
+      <c r="G46" t="n">
+        <v>38853.6884</v>
+      </c>
+      <c r="H46" t="n">
+        <v>226995.147</v>
+      </c>
+      <c r="I46" t="n">
+        <v>-3.701281025</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.0707532553</v>
+      </c>
+      <c r="K46" t="n">
+        <v>86267.20389999999</v>
+      </c>
+      <c r="L46" t="n">
+        <v>496708.8607</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.0796620503</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>2022-07</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>5.7040944936</v>
+      </c>
+      <c r="C47" t="n">
+        <v>134002.0092</v>
+      </c>
+      <c r="D47" t="n">
+        <v>892080.8789</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.1095150759</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1.9764818666</v>
+      </c>
+      <c r="G47" t="n">
+        <v>39463.5992</v>
+      </c>
+      <c r="H47" t="n">
+        <v>266458.7462</v>
+      </c>
+      <c r="I47" t="n">
+        <v>-2.9005982366</v>
+      </c>
+      <c r="J47" t="n">
+        <v>5.4852775619</v>
+      </c>
+      <c r="K47" t="n">
+        <v>86317.1367</v>
+      </c>
+      <c r="L47" t="n">
+        <v>583025.9974</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.8447577025</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>2022-08</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>-1.8171460007</v>
+      </c>
+      <c r="C48" t="n">
+        <v>132473.0136</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1024553.8925</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-0.1438443826</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-6.0823706391</v>
+      </c>
+      <c r="G48" t="n">
+        <v>38395.7146</v>
+      </c>
+      <c r="H48" t="n">
+        <v>304854.4608</v>
+      </c>
+      <c r="I48" t="n">
+        <v>-3.3131510907</v>
+      </c>
+      <c r="J48" t="n">
+        <v>-0.6874839339</v>
+      </c>
+      <c r="K48" t="n">
+        <v>85473.35340000001</v>
+      </c>
+      <c r="L48" t="n">
+        <v>668499.3508</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.646216576</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>2022-09</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1.6249588295</v>
+      </c>
+      <c r="C49" t="n">
+        <v>130899.9782</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1155453.8707</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.0534424652</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-3.5329780113</v>
+      </c>
+      <c r="G49" t="n">
+        <v>37389.548</v>
+      </c>
+      <c r="H49" t="n">
+        <v>342244.0088</v>
+      </c>
+      <c r="I49" t="n">
+        <v>-3.3372155256</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2.9621340914</v>
+      </c>
+      <c r="K49" t="n">
+        <v>84324.9026</v>
+      </c>
+      <c r="L49" t="n">
+        <v>752824.2534</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.9004313701</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>-7.3460574961</v>
+      </c>
+      <c r="C50" t="n">
+        <v>120553.6791</v>
+      </c>
+      <c r="D50" t="n">
+        <v>120553.6791</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-7.3460574961</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2.82527282</v>
+      </c>
+      <c r="G50" t="n">
+        <v>40971.6269</v>
+      </c>
+      <c r="H50" t="n">
+        <v>40971.6269</v>
+      </c>
+      <c r="I50" t="n">
+        <v>2.82527282</v>
+      </c>
+      <c r="J50" t="n">
+        <v>-3.9100029006</v>
+      </c>
+      <c r="K50" t="n">
+        <v>82775.03969999999</v>
+      </c>
+      <c r="L50" t="n">
+        <v>82775.03969999999</v>
+      </c>
+      <c r="M50" t="n">
+        <v>-3.9100029006</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>2023-02</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>14.7838892368</v>
+      </c>
+      <c r="C51" t="n">
+        <v>121321.1312</v>
+      </c>
+      <c r="D51" t="n">
+        <v>241874.8103</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2.5731995474</v>
+      </c>
+      <c r="F51" t="n">
+        <v>8.2717943249</v>
+      </c>
+      <c r="G51" t="n">
+        <v>36400.453</v>
+      </c>
+      <c r="H51" t="n">
+        <v>77372.0799</v>
+      </c>
+      <c r="I51" t="n">
+        <v>5.3177311126</v>
+      </c>
+      <c r="J51" t="n">
+        <v>11.0965133615</v>
+      </c>
+      <c r="K51" t="n">
+        <v>78864.2167</v>
+      </c>
+      <c r="L51" t="n">
+        <v>161639.2564</v>
+      </c>
+      <c r="M51" t="n">
+        <v>2.8695230996</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>2023-03</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>12.7778765523</v>
+      </c>
+      <c r="C52" t="n">
+        <v>143546.6082</v>
+      </c>
+      <c r="D52" t="n">
+        <v>385421.4185</v>
+      </c>
+      <c r="E52" t="n">
+        <v>6.1504920415</v>
+      </c>
+      <c r="F52" t="n">
+        <v>12.8382641021</v>
+      </c>
+      <c r="G52" t="n">
+        <v>41924.852</v>
+      </c>
+      <c r="H52" t="n">
+        <v>119296.9319</v>
+      </c>
+      <c r="I52" t="n">
+        <v>7.843707567</v>
+      </c>
+      <c r="J52" t="n">
+        <v>10.4271117003</v>
+      </c>
+      <c r="K52" t="n">
+        <v>93181.0333</v>
+      </c>
+      <c r="L52" t="n">
+        <v>254820.0124</v>
+      </c>
+      <c r="M52" t="n">
+        <v>5.5099618968</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>2023-04</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="C53" t="n">
+        <v>142400</v>
+      </c>
+      <c r="D53" t="n">
+        <v>527800</v>
+      </c>
+      <c r="E53" t="n">
+        <v>7.61</v>
+      </c>
+      <c r="F53" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="G53" t="n">
+        <v>41400</v>
+      </c>
+      <c r="H53" t="n">
+        <v>160700</v>
+      </c>
+      <c r="I53" t="n">
+        <v>8.119999999999999</v>
+      </c>
+      <c r="J53" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="K53" t="n">
+        <v>91400</v>
+      </c>
+      <c r="L53" t="n">
+        <v>346000</v>
+      </c>
+      <c r="M53" t="n">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>2023-05</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>9.0174515446</v>
+      </c>
+      <c r="C54" t="n">
+        <v>146741.8435</v>
+      </c>
+      <c r="D54" t="n">
+        <v>674583.233</v>
+      </c>
+      <c r="E54" t="n">
+        <v>7.9152893144</v>
+      </c>
+      <c r="F54" t="n">
+        <v>10.103415365</v>
+      </c>
+      <c r="G54" t="n">
+        <v>43511.0787</v>
+      </c>
+      <c r="H54" t="n">
+        <v>204198.0115</v>
+      </c>
+      <c r="I54" t="n">
+        <v>8.5342980859</v>
+      </c>
+      <c r="J54" t="n">
+        <v>8.8144230693</v>
+      </c>
+      <c r="K54" t="n">
+        <v>93891.1725</v>
+      </c>
+      <c r="L54" t="n">
+        <v>440097.899</v>
+      </c>
+      <c r="M54" t="n">
+        <v>7.2254464694</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>2023-06</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>8.5145531402</v>
+      </c>
+      <c r="C55" t="n">
+        <v>144296.6403</v>
+      </c>
+      <c r="D55" t="n">
+        <v>818879.8733</v>
+      </c>
+      <c r="E55" t="n">
+        <v>8.020406059300001</v>
+      </c>
+      <c r="F55" t="n">
+        <v>10.6057555143</v>
+      </c>
+      <c r="G55" t="n">
+        <v>42974.4156</v>
+      </c>
+      <c r="H55" t="n">
+        <v>247172.4271</v>
+      </c>
+      <c r="I55" t="n">
+        <v>8.8888596812</v>
+      </c>
+      <c r="J55" t="n">
+        <v>7.9072195361</v>
+      </c>
+      <c r="K55" t="n">
+        <v>93088.5411</v>
+      </c>
+      <c r="L55" t="n">
+        <v>533186.4401</v>
+      </c>
+      <c r="M55" t="n">
+        <v>7.3438551808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>